<commit_message>
update tasks and plan them on Gantt chart
</commit_message>
<xml_diff>
--- a/docs/notes/msc-timeline.xlsx
+++ b/docs/notes/msc-timeline.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7898B0C2-56BE-314E-B15A-8CDAC56F8130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3C3EC3-8040-454E-86D0-06DAA4C8E9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -258,6 +258,27 @@
   </si>
   <si>
     <t>Extract graphs</t>
+  </si>
+  <si>
+    <t>Descriptor functions</t>
+  </si>
+  <si>
+    <t>Kernels, MMD</t>
+  </si>
+  <si>
+    <t>Domain-agnostic evaluation</t>
+  </si>
+  <si>
+    <t>Domain-specific evaluation</t>
+  </si>
+  <si>
+    <t>TDA descriptors, Other metrics</t>
+  </si>
+  <si>
+    <t>Labeled edge graphs, NSPDK</t>
+  </si>
+  <si>
+    <t>Code review, conduct experiments on different datasets</t>
   </si>
 </sst>
 </file>
@@ -1318,9 +1339,6 @@
     <xf numFmtId="171" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1328,6 +1346,9 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -2115,17 +2136,17 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:FT41"/>
+  <dimension ref="A1:FT45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R20" sqref="R20"/>
+      <pane ySplit="7" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="45" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="5" customWidth="1"/>
@@ -2165,15 +2186,15 @@
       <c r="B3" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="92">
+      <c r="D3" s="93"/>
+      <c r="E3" s="95">
         <f ca="1">TODAY()</f>
-        <v>44589</v>
-      </c>
-      <c r="F3" s="92"/>
+        <v>44593</v>
+      </c>
+      <c r="F3" s="95"/>
     </row>
     <row r="4" spans="1:176" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="52"/>
@@ -2192,16 +2213,16 @@
       <c r="A5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="94"/>
+      <c r="D5" s="93"/>
       <c r="E5" s="7">
         <v>1</v>
       </c>
       <c r="I5" s="89">
         <f ca="1">I6</f>
-        <v>44585</v>
+        <v>44592</v>
       </c>
       <c r="J5" s="90"/>
       <c r="K5" s="90"/>
@@ -2211,7 +2232,7 @@
       <c r="O5" s="91"/>
       <c r="P5" s="89">
         <f ca="1">P6</f>
-        <v>44592</v>
+        <v>44599</v>
       </c>
       <c r="Q5" s="90"/>
       <c r="R5" s="90"/>
@@ -2221,7 +2242,7 @@
       <c r="V5" s="91"/>
       <c r="W5" s="89">
         <f ca="1">W6</f>
-        <v>44599</v>
+        <v>44606</v>
       </c>
       <c r="X5" s="90"/>
       <c r="Y5" s="90"/>
@@ -2231,7 +2252,7 @@
       <c r="AC5" s="91"/>
       <c r="AD5" s="89">
         <f ca="1">AD6</f>
-        <v>44606</v>
+        <v>44613</v>
       </c>
       <c r="AE5" s="90"/>
       <c r="AF5" s="90"/>
@@ -2241,7 +2262,7 @@
       <c r="AJ5" s="91"/>
       <c r="AK5" s="89">
         <f ca="1">AK6</f>
-        <v>44613</v>
+        <v>44620</v>
       </c>
       <c r="AL5" s="90"/>
       <c r="AM5" s="90"/>
@@ -2251,7 +2272,7 @@
       <c r="AQ5" s="91"/>
       <c r="AR5" s="89">
         <f ca="1">AR6</f>
-        <v>44620</v>
+        <v>44627</v>
       </c>
       <c r="AS5" s="90"/>
       <c r="AT5" s="90"/>
@@ -2261,7 +2282,7 @@
       <c r="AX5" s="91"/>
       <c r="AY5" s="89">
         <f ca="1">AY6</f>
-        <v>44627</v>
+        <v>44634</v>
       </c>
       <c r="AZ5" s="90"/>
       <c r="BA5" s="90"/>
@@ -2271,7 +2292,7 @@
       <c r="BE5" s="91"/>
       <c r="BF5" s="89">
         <f ca="1">BF6</f>
-        <v>44634</v>
+        <v>44641</v>
       </c>
       <c r="BG5" s="90"/>
       <c r="BH5" s="90"/>
@@ -2281,7 +2302,7 @@
       <c r="BL5" s="91"/>
       <c r="BM5" s="89">
         <f ca="1">BM6</f>
-        <v>44641</v>
+        <v>44648</v>
       </c>
       <c r="BN5" s="90"/>
       <c r="BO5" s="90"/>
@@ -2291,7 +2312,7 @@
       <c r="BS5" s="91"/>
       <c r="BT5" s="89">
         <f ca="1">BT6</f>
-        <v>44648</v>
+        <v>44655</v>
       </c>
       <c r="BU5" s="90"/>
       <c r="BV5" s="90"/>
@@ -2301,7 +2322,7 @@
       <c r="BZ5" s="91"/>
       <c r="CA5" s="89">
         <f ca="1">CA6</f>
-        <v>44655</v>
+        <v>44662</v>
       </c>
       <c r="CB5" s="90"/>
       <c r="CC5" s="90"/>
@@ -2311,7 +2332,7 @@
       <c r="CG5" s="91"/>
       <c r="CH5" s="89">
         <f ca="1">CH6</f>
-        <v>44662</v>
+        <v>44669</v>
       </c>
       <c r="CI5" s="90"/>
       <c r="CJ5" s="90"/>
@@ -2321,7 +2342,7 @@
       <c r="CN5" s="91"/>
       <c r="CO5" s="89">
         <f ca="1">CO6</f>
-        <v>44669</v>
+        <v>44676</v>
       </c>
       <c r="CP5" s="90"/>
       <c r="CQ5" s="90"/>
@@ -2331,7 +2352,7 @@
       <c r="CU5" s="91"/>
       <c r="CV5" s="89">
         <f ca="1">CV6</f>
-        <v>44676</v>
+        <v>44683</v>
       </c>
       <c r="CW5" s="90"/>
       <c r="CX5" s="90"/>
@@ -2341,7 +2362,7 @@
       <c r="DB5" s="91"/>
       <c r="DC5" s="89">
         <f ca="1">DC6</f>
-        <v>44683</v>
+        <v>44690</v>
       </c>
       <c r="DD5" s="90"/>
       <c r="DE5" s="90"/>
@@ -2351,7 +2372,7 @@
       <c r="DI5" s="91"/>
       <c r="DJ5" s="89">
         <f ca="1">DJ6</f>
-        <v>44690</v>
+        <v>44697</v>
       </c>
       <c r="DK5" s="90"/>
       <c r="DL5" s="90"/>
@@ -2361,7 +2382,7 @@
       <c r="DP5" s="91"/>
       <c r="DQ5" s="89">
         <f ca="1">DQ6</f>
-        <v>44697</v>
+        <v>44704</v>
       </c>
       <c r="DR5" s="90"/>
       <c r="DS5" s="90"/>
@@ -2371,7 +2392,7 @@
       <c r="DW5" s="91"/>
       <c r="DX5" s="89">
         <f ca="1">DX6</f>
-        <v>44704</v>
+        <v>44711</v>
       </c>
       <c r="DY5" s="90"/>
       <c r="DZ5" s="90"/>
@@ -2381,7 +2402,7 @@
       <c r="ED5" s="91"/>
       <c r="EE5" s="89">
         <f ca="1">EE6</f>
-        <v>44711</v>
+        <v>44718</v>
       </c>
       <c r="EF5" s="90"/>
       <c r="EG5" s="90"/>
@@ -2391,7 +2412,7 @@
       <c r="EK5" s="91"/>
       <c r="EL5" s="89">
         <f ca="1">EL6</f>
-        <v>44718</v>
+        <v>44725</v>
       </c>
       <c r="EM5" s="90"/>
       <c r="EN5" s="90"/>
@@ -2401,7 +2422,7 @@
       <c r="ER5" s="91"/>
       <c r="ES5" s="89">
         <f ca="1">ES6</f>
-        <v>44725</v>
+        <v>44732</v>
       </c>
       <c r="ET5" s="90"/>
       <c r="EU5" s="90"/>
@@ -2411,7 +2432,7 @@
       <c r="EY5" s="91"/>
       <c r="EZ5" s="89">
         <f ca="1">EZ6</f>
-        <v>44732</v>
+        <v>44739</v>
       </c>
       <c r="FA5" s="90"/>
       <c r="FB5" s="90"/>
@@ -2421,7 +2442,7 @@
       <c r="FF5" s="91"/>
       <c r="FG5" s="89">
         <f ca="1">FG6</f>
-        <v>44739</v>
+        <v>44746</v>
       </c>
       <c r="FH5" s="90"/>
       <c r="FI5" s="90"/>
@@ -2431,7 +2452,7 @@
       <c r="FM5" s="91"/>
       <c r="FN5" s="89">
         <f ca="1">FN6</f>
-        <v>44746</v>
+        <v>44753</v>
       </c>
       <c r="FO5" s="90"/>
       <c r="FP5" s="90"/>
@@ -2444,683 +2465,683 @@
       <c r="A6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
       <c r="I6" s="85">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44585</v>
+        <v>44592</v>
       </c>
       <c r="J6" s="86">
         <f ca="1">I6+1</f>
-        <v>44586</v>
+        <v>44593</v>
       </c>
       <c r="K6" s="86">
         <f t="shared" ref="K6:AX6" ca="1" si="0">J6+1</f>
-        <v>44587</v>
+        <v>44594</v>
       </c>
       <c r="L6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44588</v>
+        <v>44595</v>
       </c>
       <c r="M6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44589</v>
+        <v>44596</v>
       </c>
       <c r="N6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44590</v>
+        <v>44597</v>
       </c>
       <c r="O6" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>44591</v>
+        <v>44598</v>
       </c>
       <c r="P6" s="85">
         <f ca="1">O6+1</f>
-        <v>44592</v>
+        <v>44599</v>
       </c>
       <c r="Q6" s="86">
         <f ca="1">P6+1</f>
-        <v>44593</v>
+        <v>44600</v>
       </c>
       <c r="R6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44594</v>
+        <v>44601</v>
       </c>
       <c r="S6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44595</v>
+        <v>44602</v>
       </c>
       <c r="T6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44596</v>
+        <v>44603</v>
       </c>
       <c r="U6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44597</v>
+        <v>44604</v>
       </c>
       <c r="V6" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>44598</v>
+        <v>44605</v>
       </c>
       <c r="W6" s="85">
         <f ca="1">V6+1</f>
-        <v>44599</v>
+        <v>44606</v>
       </c>
       <c r="X6" s="86">
         <f ca="1">W6+1</f>
-        <v>44600</v>
+        <v>44607</v>
       </c>
       <c r="Y6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44601</v>
+        <v>44608</v>
       </c>
       <c r="Z6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44602</v>
+        <v>44609</v>
       </c>
       <c r="AA6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44603</v>
+        <v>44610</v>
       </c>
       <c r="AB6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44604</v>
+        <v>44611</v>
       </c>
       <c r="AC6" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>44605</v>
+        <v>44612</v>
       </c>
       <c r="AD6" s="85">
         <f ca="1">AC6+1</f>
-        <v>44606</v>
+        <v>44613</v>
       </c>
       <c r="AE6" s="86">
         <f ca="1">AD6+1</f>
-        <v>44607</v>
+        <v>44614</v>
       </c>
       <c r="AF6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44608</v>
+        <v>44615</v>
       </c>
       <c r="AG6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44609</v>
+        <v>44616</v>
       </c>
       <c r="AH6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44610</v>
+        <v>44617</v>
       </c>
       <c r="AI6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44611</v>
+        <v>44618</v>
       </c>
       <c r="AJ6" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>44612</v>
+        <v>44619</v>
       </c>
       <c r="AK6" s="85">
         <f ca="1">AJ6+1</f>
-        <v>44613</v>
+        <v>44620</v>
       </c>
       <c r="AL6" s="86">
         <f ca="1">AK6+1</f>
-        <v>44614</v>
+        <v>44621</v>
       </c>
       <c r="AM6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44615</v>
+        <v>44622</v>
       </c>
       <c r="AN6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44616</v>
+        <v>44623</v>
       </c>
       <c r="AO6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44617</v>
+        <v>44624</v>
       </c>
       <c r="AP6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44618</v>
+        <v>44625</v>
       </c>
       <c r="AQ6" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>44619</v>
+        <v>44626</v>
       </c>
       <c r="AR6" s="85">
         <f ca="1">AQ6+1</f>
-        <v>44620</v>
+        <v>44627</v>
       </c>
       <c r="AS6" s="86">
         <f ca="1">AR6+1</f>
-        <v>44621</v>
+        <v>44628</v>
       </c>
       <c r="AT6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44622</v>
+        <v>44629</v>
       </c>
       <c r="AU6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44623</v>
+        <v>44630</v>
       </c>
       <c r="AV6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44624</v>
+        <v>44631</v>
       </c>
       <c r="AW6" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>44625</v>
+        <v>44632</v>
       </c>
       <c r="AX6" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>44626</v>
+        <v>44633</v>
       </c>
       <c r="AY6" s="85">
         <f ca="1">AX6+1</f>
-        <v>44627</v>
+        <v>44634</v>
       </c>
       <c r="AZ6" s="86">
         <f ca="1">AY6+1</f>
-        <v>44628</v>
+        <v>44635</v>
       </c>
       <c r="BA6" s="86">
         <f t="shared" ref="BA6:BE6" ca="1" si="1">AZ6+1</f>
-        <v>44629</v>
+        <v>44636</v>
       </c>
       <c r="BB6" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>44630</v>
+        <v>44637</v>
       </c>
       <c r="BC6" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>44631</v>
+        <v>44638</v>
       </c>
       <c r="BD6" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>44632</v>
+        <v>44639</v>
       </c>
       <c r="BE6" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>44633</v>
+        <v>44640</v>
       </c>
       <c r="BF6" s="85">
         <f ca="1">BE6+1</f>
-        <v>44634</v>
+        <v>44641</v>
       </c>
       <c r="BG6" s="86">
         <f ca="1">BF6+1</f>
-        <v>44635</v>
+        <v>44642</v>
       </c>
       <c r="BH6" s="86">
         <f t="shared" ref="BH6:BL6" ca="1" si="2">BG6+1</f>
-        <v>44636</v>
+        <v>44643</v>
       </c>
       <c r="BI6" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>44637</v>
+        <v>44644</v>
       </c>
       <c r="BJ6" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>44638</v>
+        <v>44645</v>
       </c>
       <c r="BK6" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>44639</v>
+        <v>44646</v>
       </c>
       <c r="BL6" s="87">
         <f t="shared" ca="1" si="2"/>
-        <v>44640</v>
+        <v>44647</v>
       </c>
       <c r="BM6" s="85">
         <f ca="1">BL6+1</f>
-        <v>44641</v>
+        <v>44648</v>
       </c>
       <c r="BN6" s="86">
         <f ca="1">BM6+1</f>
-        <v>44642</v>
+        <v>44649</v>
       </c>
       <c r="BO6" s="86">
         <f t="shared" ref="BO6" ca="1" si="3">BN6+1</f>
-        <v>44643</v>
+        <v>44650</v>
       </c>
       <c r="BP6" s="86">
         <f t="shared" ref="BP6" ca="1" si="4">BO6+1</f>
-        <v>44644</v>
+        <v>44651</v>
       </c>
       <c r="BQ6" s="86">
         <f t="shared" ref="BQ6" ca="1" si="5">BP6+1</f>
-        <v>44645</v>
+        <v>44652</v>
       </c>
       <c r="BR6" s="86">
         <f t="shared" ref="BR6" ca="1" si="6">BQ6+1</f>
-        <v>44646</v>
+        <v>44653</v>
       </c>
       <c r="BS6" s="87">
         <f t="shared" ref="BS6" ca="1" si="7">BR6+1</f>
-        <v>44647</v>
+        <v>44654</v>
       </c>
       <c r="BT6" s="85">
         <f ca="1">BS6+1</f>
-        <v>44648</v>
+        <v>44655</v>
       </c>
       <c r="BU6" s="86">
         <f ca="1">BT6+1</f>
-        <v>44649</v>
+        <v>44656</v>
       </c>
       <c r="BV6" s="86">
         <f t="shared" ref="BV6" ca="1" si="8">BU6+1</f>
-        <v>44650</v>
+        <v>44657</v>
       </c>
       <c r="BW6" s="86">
         <f t="shared" ref="BW6" ca="1" si="9">BV6+1</f>
-        <v>44651</v>
+        <v>44658</v>
       </c>
       <c r="BX6" s="86">
         <f t="shared" ref="BX6" ca="1" si="10">BW6+1</f>
-        <v>44652</v>
+        <v>44659</v>
       </c>
       <c r="BY6" s="86">
         <f t="shared" ref="BY6" ca="1" si="11">BX6+1</f>
-        <v>44653</v>
+        <v>44660</v>
       </c>
       <c r="BZ6" s="87">
         <f t="shared" ref="BZ6" ca="1" si="12">BY6+1</f>
-        <v>44654</v>
+        <v>44661</v>
       </c>
       <c r="CA6" s="85">
         <f ca="1">BZ6+1</f>
-        <v>44655</v>
+        <v>44662</v>
       </c>
       <c r="CB6" s="86">
         <f ca="1">CA6+1</f>
-        <v>44656</v>
+        <v>44663</v>
       </c>
       <c r="CC6" s="86">
         <f t="shared" ref="CC6" ca="1" si="13">CB6+1</f>
-        <v>44657</v>
+        <v>44664</v>
       </c>
       <c r="CD6" s="86">
         <f t="shared" ref="CD6" ca="1" si="14">CC6+1</f>
-        <v>44658</v>
+        <v>44665</v>
       </c>
       <c r="CE6" s="86">
         <f t="shared" ref="CE6" ca="1" si="15">CD6+1</f>
-        <v>44659</v>
+        <v>44666</v>
       </c>
       <c r="CF6" s="86">
         <f t="shared" ref="CF6" ca="1" si="16">CE6+1</f>
-        <v>44660</v>
+        <v>44667</v>
       </c>
       <c r="CG6" s="87">
         <f t="shared" ref="CG6" ca="1" si="17">CF6+1</f>
-        <v>44661</v>
+        <v>44668</v>
       </c>
       <c r="CH6" s="85">
         <f ca="1">CG6+1</f>
-        <v>44662</v>
+        <v>44669</v>
       </c>
       <c r="CI6" s="86">
         <f ca="1">CH6+1</f>
-        <v>44663</v>
+        <v>44670</v>
       </c>
       <c r="CJ6" s="86">
         <f t="shared" ref="CJ6" ca="1" si="18">CI6+1</f>
-        <v>44664</v>
+        <v>44671</v>
       </c>
       <c r="CK6" s="86">
         <f t="shared" ref="CK6" ca="1" si="19">CJ6+1</f>
-        <v>44665</v>
+        <v>44672</v>
       </c>
       <c r="CL6" s="86">
         <f t="shared" ref="CL6" ca="1" si="20">CK6+1</f>
-        <v>44666</v>
+        <v>44673</v>
       </c>
       <c r="CM6" s="86">
         <f t="shared" ref="CM6" ca="1" si="21">CL6+1</f>
-        <v>44667</v>
+        <v>44674</v>
       </c>
       <c r="CN6" s="87">
         <f t="shared" ref="CN6" ca="1" si="22">CM6+1</f>
-        <v>44668</v>
+        <v>44675</v>
       </c>
       <c r="CO6" s="85">
         <f ca="1">CN6+1</f>
-        <v>44669</v>
+        <v>44676</v>
       </c>
       <c r="CP6" s="86">
         <f ca="1">CO6+1</f>
-        <v>44670</v>
+        <v>44677</v>
       </c>
       <c r="CQ6" s="86">
         <f t="shared" ref="CQ6" ca="1" si="23">CP6+1</f>
-        <v>44671</v>
+        <v>44678</v>
       </c>
       <c r="CR6" s="86">
         <f t="shared" ref="CR6" ca="1" si="24">CQ6+1</f>
-        <v>44672</v>
+        <v>44679</v>
       </c>
       <c r="CS6" s="86">
         <f t="shared" ref="CS6" ca="1" si="25">CR6+1</f>
-        <v>44673</v>
+        <v>44680</v>
       </c>
       <c r="CT6" s="86">
         <f t="shared" ref="CT6" ca="1" si="26">CS6+1</f>
-        <v>44674</v>
+        <v>44681</v>
       </c>
       <c r="CU6" s="87">
         <f t="shared" ref="CU6" ca="1" si="27">CT6+1</f>
-        <v>44675</v>
+        <v>44682</v>
       </c>
       <c r="CV6" s="85">
         <f ca="1">CU6+1</f>
-        <v>44676</v>
+        <v>44683</v>
       </c>
       <c r="CW6" s="86">
         <f ca="1">CV6+1</f>
-        <v>44677</v>
+        <v>44684</v>
       </c>
       <c r="CX6" s="86">
         <f t="shared" ref="CX6" ca="1" si="28">CW6+1</f>
-        <v>44678</v>
+        <v>44685</v>
       </c>
       <c r="CY6" s="86">
         <f t="shared" ref="CY6" ca="1" si="29">CX6+1</f>
-        <v>44679</v>
+        <v>44686</v>
       </c>
       <c r="CZ6" s="86">
         <f t="shared" ref="CZ6" ca="1" si="30">CY6+1</f>
-        <v>44680</v>
+        <v>44687</v>
       </c>
       <c r="DA6" s="86">
         <f t="shared" ref="DA6" ca="1" si="31">CZ6+1</f>
-        <v>44681</v>
+        <v>44688</v>
       </c>
       <c r="DB6" s="87">
         <f t="shared" ref="DB6" ca="1" si="32">DA6+1</f>
-        <v>44682</v>
+        <v>44689</v>
       </c>
       <c r="DC6" s="85">
         <f ca="1">DB6+1</f>
-        <v>44683</v>
+        <v>44690</v>
       </c>
       <c r="DD6" s="86">
         <f ca="1">DC6+1</f>
-        <v>44684</v>
+        <v>44691</v>
       </c>
       <c r="DE6" s="86">
         <f t="shared" ref="DE6" ca="1" si="33">DD6+1</f>
-        <v>44685</v>
+        <v>44692</v>
       </c>
       <c r="DF6" s="86">
         <f t="shared" ref="DF6" ca="1" si="34">DE6+1</f>
-        <v>44686</v>
+        <v>44693</v>
       </c>
       <c r="DG6" s="86">
         <f t="shared" ref="DG6" ca="1" si="35">DF6+1</f>
-        <v>44687</v>
+        <v>44694</v>
       </c>
       <c r="DH6" s="86">
         <f t="shared" ref="DH6" ca="1" si="36">DG6+1</f>
-        <v>44688</v>
+        <v>44695</v>
       </c>
       <c r="DI6" s="87">
         <f t="shared" ref="DI6" ca="1" si="37">DH6+1</f>
-        <v>44689</v>
+        <v>44696</v>
       </c>
       <c r="DJ6" s="85">
         <f ca="1">DI6+1</f>
-        <v>44690</v>
+        <v>44697</v>
       </c>
       <c r="DK6" s="86">
         <f ca="1">DJ6+1</f>
-        <v>44691</v>
+        <v>44698</v>
       </c>
       <c r="DL6" s="86">
         <f t="shared" ref="DL6" ca="1" si="38">DK6+1</f>
-        <v>44692</v>
+        <v>44699</v>
       </c>
       <c r="DM6" s="86">
         <f t="shared" ref="DM6" ca="1" si="39">DL6+1</f>
-        <v>44693</v>
+        <v>44700</v>
       </c>
       <c r="DN6" s="86">
         <f t="shared" ref="DN6" ca="1" si="40">DM6+1</f>
-        <v>44694</v>
+        <v>44701</v>
       </c>
       <c r="DO6" s="86">
         <f t="shared" ref="DO6" ca="1" si="41">DN6+1</f>
-        <v>44695</v>
+        <v>44702</v>
       </c>
       <c r="DP6" s="87">
         <f t="shared" ref="DP6" ca="1" si="42">DO6+1</f>
-        <v>44696</v>
+        <v>44703</v>
       </c>
       <c r="DQ6" s="85">
         <f ca="1">DP6+1</f>
-        <v>44697</v>
+        <v>44704</v>
       </c>
       <c r="DR6" s="86">
         <f ca="1">DQ6+1</f>
-        <v>44698</v>
+        <v>44705</v>
       </c>
       <c r="DS6" s="86">
         <f t="shared" ref="DS6" ca="1" si="43">DR6+1</f>
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="DT6" s="86">
         <f t="shared" ref="DT6" ca="1" si="44">DS6+1</f>
-        <v>44700</v>
+        <v>44707</v>
       </c>
       <c r="DU6" s="86">
         <f t="shared" ref="DU6" ca="1" si="45">DT6+1</f>
-        <v>44701</v>
+        <v>44708</v>
       </c>
       <c r="DV6" s="86">
         <f t="shared" ref="DV6" ca="1" si="46">DU6+1</f>
-        <v>44702</v>
+        <v>44709</v>
       </c>
       <c r="DW6" s="87">
         <f t="shared" ref="DW6" ca="1" si="47">DV6+1</f>
-        <v>44703</v>
+        <v>44710</v>
       </c>
       <c r="DX6" s="85">
         <f ca="1">DW6+1</f>
-        <v>44704</v>
+        <v>44711</v>
       </c>
       <c r="DY6" s="86">
         <f ca="1">DX6+1</f>
-        <v>44705</v>
+        <v>44712</v>
       </c>
       <c r="DZ6" s="86">
         <f t="shared" ref="DZ6" ca="1" si="48">DY6+1</f>
-        <v>44706</v>
+        <v>44713</v>
       </c>
       <c r="EA6" s="86">
         <f t="shared" ref="EA6" ca="1" si="49">DZ6+1</f>
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="EB6" s="86">
         <f t="shared" ref="EB6" ca="1" si="50">EA6+1</f>
-        <v>44708</v>
+        <v>44715</v>
       </c>
       <c r="EC6" s="86">
         <f t="shared" ref="EC6" ca="1" si="51">EB6+1</f>
-        <v>44709</v>
+        <v>44716</v>
       </c>
       <c r="ED6" s="87">
         <f t="shared" ref="ED6" ca="1" si="52">EC6+1</f>
-        <v>44710</v>
+        <v>44717</v>
       </c>
       <c r="EE6" s="85">
         <f ca="1">ED6+1</f>
-        <v>44711</v>
+        <v>44718</v>
       </c>
       <c r="EF6" s="86">
         <f ca="1">EE6+1</f>
-        <v>44712</v>
+        <v>44719</v>
       </c>
       <c r="EG6" s="86">
         <f t="shared" ref="EG6" ca="1" si="53">EF6+1</f>
-        <v>44713</v>
+        <v>44720</v>
       </c>
       <c r="EH6" s="86">
         <f t="shared" ref="EH6" ca="1" si="54">EG6+1</f>
-        <v>44714</v>
+        <v>44721</v>
       </c>
       <c r="EI6" s="86">
         <f t="shared" ref="EI6" ca="1" si="55">EH6+1</f>
-        <v>44715</v>
+        <v>44722</v>
       </c>
       <c r="EJ6" s="86">
         <f t="shared" ref="EJ6" ca="1" si="56">EI6+1</f>
-        <v>44716</v>
+        <v>44723</v>
       </c>
       <c r="EK6" s="87">
         <f t="shared" ref="EK6" ca="1" si="57">EJ6+1</f>
-        <v>44717</v>
+        <v>44724</v>
       </c>
       <c r="EL6" s="85">
         <f ca="1">EK6+1</f>
-        <v>44718</v>
+        <v>44725</v>
       </c>
       <c r="EM6" s="86">
         <f ca="1">EL6+1</f>
-        <v>44719</v>
+        <v>44726</v>
       </c>
       <c r="EN6" s="86">
         <f t="shared" ref="EN6" ca="1" si="58">EM6+1</f>
-        <v>44720</v>
+        <v>44727</v>
       </c>
       <c r="EO6" s="86">
         <f t="shared" ref="EO6" ca="1" si="59">EN6+1</f>
-        <v>44721</v>
+        <v>44728</v>
       </c>
       <c r="EP6" s="86">
         <f t="shared" ref="EP6" ca="1" si="60">EO6+1</f>
-        <v>44722</v>
+        <v>44729</v>
       </c>
       <c r="EQ6" s="86">
         <f t="shared" ref="EQ6" ca="1" si="61">EP6+1</f>
-        <v>44723</v>
+        <v>44730</v>
       </c>
       <c r="ER6" s="87">
         <f t="shared" ref="ER6" ca="1" si="62">EQ6+1</f>
-        <v>44724</v>
+        <v>44731</v>
       </c>
       <c r="ES6" s="85">
         <f ca="1">ER6+1</f>
-        <v>44725</v>
+        <v>44732</v>
       </c>
       <c r="ET6" s="86">
         <f ca="1">ES6+1</f>
-        <v>44726</v>
+        <v>44733</v>
       </c>
       <c r="EU6" s="86">
         <f t="shared" ref="EU6" ca="1" si="63">ET6+1</f>
-        <v>44727</v>
+        <v>44734</v>
       </c>
       <c r="EV6" s="86">
         <f t="shared" ref="EV6" ca="1" si="64">EU6+1</f>
-        <v>44728</v>
+        <v>44735</v>
       </c>
       <c r="EW6" s="86">
         <f t="shared" ref="EW6" ca="1" si="65">EV6+1</f>
-        <v>44729</v>
+        <v>44736</v>
       </c>
       <c r="EX6" s="86">
         <f t="shared" ref="EX6" ca="1" si="66">EW6+1</f>
-        <v>44730</v>
+        <v>44737</v>
       </c>
       <c r="EY6" s="87">
         <f t="shared" ref="EY6" ca="1" si="67">EX6+1</f>
-        <v>44731</v>
+        <v>44738</v>
       </c>
       <c r="EZ6" s="85">
         <f ca="1">EY6+1</f>
-        <v>44732</v>
+        <v>44739</v>
       </c>
       <c r="FA6" s="86">
         <f ca="1">EZ6+1</f>
-        <v>44733</v>
+        <v>44740</v>
       </c>
       <c r="FB6" s="86">
         <f t="shared" ref="FB6" ca="1" si="68">FA6+1</f>
-        <v>44734</v>
+        <v>44741</v>
       </c>
       <c r="FC6" s="86">
         <f t="shared" ref="FC6" ca="1" si="69">FB6+1</f>
-        <v>44735</v>
+        <v>44742</v>
       </c>
       <c r="FD6" s="86">
         <f t="shared" ref="FD6" ca="1" si="70">FC6+1</f>
-        <v>44736</v>
+        <v>44743</v>
       </c>
       <c r="FE6" s="86">
         <f t="shared" ref="FE6" ca="1" si="71">FD6+1</f>
-        <v>44737</v>
+        <v>44744</v>
       </c>
       <c r="FF6" s="87">
         <f t="shared" ref="FF6" ca="1" si="72">FE6+1</f>
-        <v>44738</v>
+        <v>44745</v>
       </c>
       <c r="FG6" s="85">
         <f ca="1">FF6+1</f>
-        <v>44739</v>
+        <v>44746</v>
       </c>
       <c r="FH6" s="86">
         <f ca="1">FG6+1</f>
-        <v>44740</v>
+        <v>44747</v>
       </c>
       <c r="FI6" s="86">
         <f t="shared" ref="FI6" ca="1" si="73">FH6+1</f>
-        <v>44741</v>
+        <v>44748</v>
       </c>
       <c r="FJ6" s="86">
         <f t="shared" ref="FJ6" ca="1" si="74">FI6+1</f>
-        <v>44742</v>
+        <v>44749</v>
       </c>
       <c r="FK6" s="86">
         <f t="shared" ref="FK6" ca="1" si="75">FJ6+1</f>
-        <v>44743</v>
+        <v>44750</v>
       </c>
       <c r="FL6" s="86">
         <f t="shared" ref="FL6" ca="1" si="76">FK6+1</f>
-        <v>44744</v>
+        <v>44751</v>
       </c>
       <c r="FM6" s="87">
         <f t="shared" ref="FM6" ca="1" si="77">FL6+1</f>
-        <v>44745</v>
+        <v>44752</v>
       </c>
       <c r="FN6" s="85">
         <f ca="1">FM6+1</f>
-        <v>44746</v>
+        <v>44753</v>
       </c>
       <c r="FO6" s="86">
         <f ca="1">FN6+1</f>
-        <v>44747</v>
+        <v>44754</v>
       </c>
       <c r="FP6" s="86">
         <f t="shared" ref="FP6" ca="1" si="78">FO6+1</f>
-        <v>44748</v>
+        <v>44755</v>
       </c>
       <c r="FQ6" s="86">
         <f t="shared" ref="FQ6" ca="1" si="79">FP6+1</f>
-        <v>44749</v>
+        <v>44756</v>
       </c>
       <c r="FR6" s="86">
         <f t="shared" ref="FR6" ca="1" si="80">FQ6+1</f>
-        <v>44750</v>
+        <v>44757</v>
       </c>
       <c r="FS6" s="86">
         <f t="shared" ref="FS6" ca="1" si="81">FR6+1</f>
-        <v>44751</v>
+        <v>44758</v>
       </c>
       <c r="FT6" s="87">
         <f t="shared" ref="FT6" ca="1" si="82">FS6+1</f>
-        <v>44752</v>
+        <v>44759</v>
       </c>
     </row>
     <row r="7" spans="1:176" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4009,7 +4030,7 @@
       <c r="F9" s="68"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="str">
-        <f t="shared" ref="H9:H38" si="89">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H9:H42" si="89">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I9" s="31"/>
@@ -5479,12 +5500,12 @@
         <v>44588</v>
       </c>
       <c r="F17" s="81">
-        <v>44591</v>
+        <v>44605</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14">
         <f t="shared" si="89"/>
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
@@ -5657,15 +5678,21 @@
     </row>
     <row r="18" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
-      <c r="B18" s="63"/>
+      <c r="B18" s="63" t="s">
+        <v>60</v>
+      </c>
       <c r="C18" s="56"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
+      <c r="E18" s="81">
+        <v>44606</v>
+      </c>
+      <c r="F18" s="81">
+        <v>44612</v>
+      </c>
       <c r="G18" s="14"/>
-      <c r="H18" s="14" t="str">
+      <c r="H18" s="14">
         <f t="shared" si="89"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
@@ -5838,15 +5865,21 @@
     </row>
     <row r="19" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45"/>
-      <c r="B19" s="63"/>
+      <c r="B19" s="63" t="s">
+        <v>61</v>
+      </c>
       <c r="C19" s="56"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
+      <c r="E19" s="81">
+        <v>44613</v>
+      </c>
+      <c r="F19" s="81">
+        <v>44619</v>
+      </c>
       <c r="G19" s="14"/>
-      <c r="H19" s="14" t="str">
+      <c r="H19" s="14">
         <f t="shared" si="89"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
@@ -6019,16 +6052,19 @@
     </row>
     <row r="20" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="45"/>
-      <c r="B20" s="63"/>
+      <c r="B20" s="63" t="s">
+        <v>62</v>
+      </c>
       <c r="C20" s="56"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
+      <c r="E20" s="81">
+        <v>44620</v>
+      </c>
+      <c r="F20" s="81">
+        <v>44626</v>
+      </c>
       <c r="G20" s="14"/>
-      <c r="H20" s="14" t="str">
-        <f t="shared" si="89"/>
-        <v/>
-      </c>
+      <c r="H20" s="14"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
@@ -6045,7 +6081,7 @@
       <c r="V20" s="31"/>
       <c r="W20" s="31"/>
       <c r="X20" s="31"/>
-      <c r="Y20" s="31"/>
+      <c r="Y20" s="32"/>
       <c r="Z20" s="31"/>
       <c r="AA20" s="31"/>
       <c r="AB20" s="31"/>
@@ -6199,21 +6235,20 @@
       <c r="FT20" s="31"/>
     </row>
     <row r="21" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="72"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="56"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="81">
+        <v>44627</v>
+      </c>
+      <c r="F21" s="81">
+        <v>44640</v>
+      </c>
       <c r="G21" s="14"/>
-      <c r="H21" s="14" t="str">
-        <f t="shared" si="89"/>
-        <v/>
-      </c>
+      <c r="H21" s="14"/>
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
@@ -6230,7 +6265,7 @@
       <c r="V21" s="31"/>
       <c r="W21" s="31"/>
       <c r="X21" s="31"/>
-      <c r="Y21" s="31"/>
+      <c r="Y21" s="32"/>
       <c r="Z21" s="31"/>
       <c r="AA21" s="31"/>
       <c r="AB21" s="31"/>
@@ -6385,18 +6420,19 @@
     </row>
     <row r="22" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
-      <c r="B22" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
+      <c r="B22" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="56"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="81">
+        <v>44641</v>
+      </c>
+      <c r="F22" s="81">
+        <v>44654</v>
+      </c>
       <c r="G22" s="14"/>
-      <c r="H22" s="14" t="str">
-        <f t="shared" si="89"/>
-        <v/>
-      </c>
+      <c r="H22" s="14"/>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
@@ -6413,7 +6449,7 @@
       <c r="V22" s="31"/>
       <c r="W22" s="31"/>
       <c r="X22" s="31"/>
-      <c r="Y22" s="31"/>
+      <c r="Y22" s="32"/>
       <c r="Z22" s="31"/>
       <c r="AA22" s="31"/>
       <c r="AB22" s="31"/>
@@ -6568,18 +6604,19 @@
     </row>
     <row r="23" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="45"/>
-      <c r="B23" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
+      <c r="B23" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="56"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="81">
+        <v>44655</v>
+      </c>
+      <c r="F23" s="81">
+        <v>44661</v>
+      </c>
       <c r="G23" s="14"/>
-      <c r="H23" s="14" t="str">
-        <f t="shared" si="89"/>
-        <v/>
-      </c>
+      <c r="H23" s="14"/>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
@@ -6596,7 +6633,7 @@
       <c r="V23" s="31"/>
       <c r="W23" s="31"/>
       <c r="X23" s="31"/>
-      <c r="Y23" s="31"/>
+      <c r="Y23" s="32"/>
       <c r="Z23" s="31"/>
       <c r="AA23" s="31"/>
       <c r="AB23" s="31"/>
@@ -6751,15 +6788,21 @@
     </row>
     <row r="24" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
+      <c r="B24" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="56"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="81">
+        <v>44662</v>
+      </c>
+      <c r="F24" s="81">
+        <v>44675</v>
+      </c>
       <c r="G24" s="14"/>
-      <c r="H24" s="14" t="str">
+      <c r="H24" s="14">
         <f t="shared" si="89"/>
-        <v/>
+        <v>14</v>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -6931,12 +6974,16 @@
       <c r="FT24" s="31"/>
     </row>
     <row r="25" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
+      <c r="A25" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14" t="str">
         <f t="shared" si="89"/>
@@ -7113,7 +7160,9 @@
     </row>
     <row r="26" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="45"/>
-      <c r="B26" s="64"/>
+      <c r="B26" s="64" t="s">
+        <v>48</v>
+      </c>
       <c r="C26" s="58"/>
       <c r="D26" s="23"/>
       <c r="E26" s="82"/>
@@ -7293,16 +7342,14 @@
       <c r="FT26" s="31"/>
     </row>
     <row r="27" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="74"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="58"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14" t="str">
         <f t="shared" si="89"/>
@@ -7479,21 +7526,15 @@
     </row>
     <row r="28" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
-      <c r="B28" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="83">
-        <v>44723</v>
-      </c>
-      <c r="F28" s="83">
-        <v>44729</v>
-      </c>
+      <c r="B28" s="64"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
       <c r="G28" s="14"/>
-      <c r="H28" s="14">
+      <c r="H28" s="14" t="str">
         <f t="shared" si="89"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -7666,19 +7707,16 @@
     </row>
     <row r="29" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
-      <c r="B29" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="83">
-        <v>44725</v>
-      </c>
-      <c r="F29" s="83">
-        <v>44729</v>
-      </c>
+      <c r="B29" s="64"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="H29" s="14" t="str">
+        <f t="shared" si="89"/>
+        <v/>
+      </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
       <c r="K29" s="31"/>
@@ -7850,19 +7888,16 @@
     </row>
     <row r="30" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
-      <c r="B30" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="83">
-        <v>44718</v>
-      </c>
-      <c r="F30" s="83">
-        <v>44724</v>
-      </c>
+      <c r="B30" s="64"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="H30" s="14" t="str">
+        <f t="shared" si="89"/>
+        <v/>
+      </c>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
       <c r="K30" s="31"/>
@@ -8033,20 +8068,21 @@
       <c r="FT30" s="31"/>
     </row>
     <row r="31" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
-      <c r="B31" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="60"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="83">
-        <v>44718</v>
-      </c>
-      <c r="F31" s="83">
-        <v>44724</v>
-      </c>
+      <c r="A31" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="59"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="H31" s="14" t="str">
+        <f t="shared" si="89"/>
+        <v/>
+      </c>
       <c r="I31" s="31"/>
       <c r="J31" s="31"/>
       <c r="K31" s="31"/>
@@ -8219,18 +8255,21 @@
     <row r="32" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="45"/>
       <c r="B32" s="65" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C32" s="60"/>
       <c r="D32" s="26"/>
       <c r="E32" s="83">
-        <v>44725</v>
+        <v>44669</v>
       </c>
       <c r="F32" s="83">
-        <v>44729</v>
+        <v>44675</v>
       </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="H32" s="14">
+        <f t="shared" si="89"/>
+        <v>7</v>
+      </c>
       <c r="I32" s="31"/>
       <c r="J32" s="31"/>
       <c r="K32" s="31"/>
@@ -8403,21 +8442,18 @@
     <row r="33" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="45"/>
       <c r="B33" s="65" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C33" s="60"/>
       <c r="D33" s="26"/>
       <c r="E33" s="83">
+        <v>44725</v>
+      </c>
+      <c r="F33" s="83">
         <v>44729</v>
       </c>
-      <c r="F33" s="83">
-        <v>44731</v>
-      </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="14">
-        <f t="shared" si="89"/>
-        <v>3</v>
-      </c>
+      <c r="H33" s="14"/>
       <c r="I33" s="31"/>
       <c r="J33" s="31"/>
       <c r="K33" s="31"/>
@@ -8590,21 +8626,18 @@
     <row r="34" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="45"/>
       <c r="B34" s="65" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C34" s="60"/>
       <c r="D34" s="26"/>
       <c r="E34" s="83">
-        <v>44732</v>
+        <v>44718</v>
       </c>
       <c r="F34" s="83">
-        <v>44738</v>
+        <v>44724</v>
       </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="14">
-        <f t="shared" si="89"/>
-        <v>7</v>
-      </c>
+      <c r="H34" s="14"/>
       <c r="I34" s="31"/>
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
@@ -8777,21 +8810,18 @@
     <row r="35" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="45"/>
       <c r="B35" s="65" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C35" s="60"/>
       <c r="D35" s="26"/>
       <c r="E35" s="83">
-        <v>44739</v>
+        <v>44718</v>
       </c>
       <c r="F35" s="83">
-        <v>44745</v>
+        <v>44724</v>
       </c>
       <c r="G35" s="14"/>
-      <c r="H35" s="14">
-        <f t="shared" si="89"/>
-        <v>7</v>
-      </c>
+      <c r="H35" s="14"/>
       <c r="I35" s="31"/>
       <c r="J35" s="31"/>
       <c r="K35" s="31"/>
@@ -8964,21 +8994,18 @@
     <row r="36" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="45"/>
       <c r="B36" s="65" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C36" s="60"/>
       <c r="D36" s="26"/>
       <c r="E36" s="83">
-        <v>44746</v>
+        <v>44725</v>
       </c>
       <c r="F36" s="83">
-        <v>44752</v>
+        <v>44729</v>
       </c>
       <c r="G36" s="14"/>
-      <c r="H36" s="14">
-        <f t="shared" si="89"/>
-        <v>7</v>
-      </c>
+      <c r="H36" s="14"/>
       <c r="I36" s="31"/>
       <c r="J36" s="31"/>
       <c r="K36" s="31"/>
@@ -9149,18 +9176,22 @@
       <c r="FT36" s="31"/>
     </row>
     <row r="37" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="60"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="83">
+        <v>44729</v>
+      </c>
+      <c r="F37" s="83">
+        <v>44731</v>
+      </c>
       <c r="G37" s="14"/>
-      <c r="H37" s="14" t="str">
+      <c r="H37" s="14">
         <f t="shared" si="89"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="I37" s="31"/>
       <c r="J37" s="31"/>
@@ -9332,223 +9363,946 @@
       <c r="FT37" s="31"/>
     </row>
     <row r="38" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30" t="str">
+      <c r="A38" s="45"/>
+      <c r="B38" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="60"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="83">
+        <v>44732</v>
+      </c>
+      <c r="F38" s="83">
+        <v>44738</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14">
+        <f t="shared" si="89"/>
+        <v>7</v>
+      </c>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
+      <c r="Z38" s="31"/>
+      <c r="AA38" s="31"/>
+      <c r="AB38" s="31"/>
+      <c r="AC38" s="31"/>
+      <c r="AD38" s="31"/>
+      <c r="AE38" s="31"/>
+      <c r="AF38" s="31"/>
+      <c r="AG38" s="31"/>
+      <c r="AH38" s="31"/>
+      <c r="AI38" s="31"/>
+      <c r="AJ38" s="31"/>
+      <c r="AK38" s="31"/>
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+      <c r="AO38" s="31"/>
+      <c r="AP38" s="31"/>
+      <c r="AQ38" s="31"/>
+      <c r="AR38" s="31"/>
+      <c r="AS38" s="31"/>
+      <c r="AT38" s="31"/>
+      <c r="AU38" s="31"/>
+      <c r="AV38" s="31"/>
+      <c r="AW38" s="31"/>
+      <c r="AX38" s="31"/>
+      <c r="AY38" s="31"/>
+      <c r="AZ38" s="31"/>
+      <c r="BA38" s="31"/>
+      <c r="BB38" s="31"/>
+      <c r="BC38" s="31"/>
+      <c r="BD38" s="31"/>
+      <c r="BE38" s="31"/>
+      <c r="BF38" s="31"/>
+      <c r="BG38" s="31"/>
+      <c r="BH38" s="31"/>
+      <c r="BI38" s="31"/>
+      <c r="BJ38" s="31"/>
+      <c r="BK38" s="31"/>
+      <c r="BL38" s="31"/>
+      <c r="BM38" s="31"/>
+      <c r="BN38" s="31"/>
+      <c r="BO38" s="31"/>
+      <c r="BP38" s="31"/>
+      <c r="BQ38" s="31"/>
+      <c r="BR38" s="31"/>
+      <c r="BS38" s="31"/>
+      <c r="BT38" s="31"/>
+      <c r="BU38" s="31"/>
+      <c r="BV38" s="31"/>
+      <c r="BW38" s="31"/>
+      <c r="BX38" s="31"/>
+      <c r="BY38" s="31"/>
+      <c r="BZ38" s="31"/>
+      <c r="CA38" s="31"/>
+      <c r="CB38" s="31"/>
+      <c r="CC38" s="31"/>
+      <c r="CD38" s="31"/>
+      <c r="CE38" s="31"/>
+      <c r="CF38" s="31"/>
+      <c r="CG38" s="31"/>
+      <c r="CH38" s="31"/>
+      <c r="CI38" s="31"/>
+      <c r="CJ38" s="31"/>
+      <c r="CK38" s="31"/>
+      <c r="CL38" s="31"/>
+      <c r="CM38" s="31"/>
+      <c r="CN38" s="31"/>
+      <c r="CO38" s="31"/>
+      <c r="CP38" s="31"/>
+      <c r="CQ38" s="31"/>
+      <c r="CR38" s="31"/>
+      <c r="CS38" s="31"/>
+      <c r="CT38" s="31"/>
+      <c r="CU38" s="31"/>
+      <c r="CV38" s="31"/>
+      <c r="CW38" s="31"/>
+      <c r="CX38" s="31"/>
+      <c r="CY38" s="31"/>
+      <c r="CZ38" s="31"/>
+      <c r="DA38" s="31"/>
+      <c r="DB38" s="31"/>
+      <c r="DC38" s="31"/>
+      <c r="DD38" s="31"/>
+      <c r="DE38" s="31"/>
+      <c r="DF38" s="31"/>
+      <c r="DG38" s="31"/>
+      <c r="DH38" s="31"/>
+      <c r="DI38" s="31"/>
+      <c r="DJ38" s="31"/>
+      <c r="DK38" s="31"/>
+      <c r="DL38" s="31"/>
+      <c r="DM38" s="31"/>
+      <c r="DN38" s="31"/>
+      <c r="DO38" s="31"/>
+      <c r="DP38" s="31"/>
+      <c r="DQ38" s="31"/>
+      <c r="DR38" s="31"/>
+      <c r="DS38" s="31"/>
+      <c r="DT38" s="31"/>
+      <c r="DU38" s="31"/>
+      <c r="DV38" s="31"/>
+      <c r="DW38" s="31"/>
+      <c r="DX38" s="31"/>
+      <c r="DY38" s="31"/>
+      <c r="DZ38" s="31"/>
+      <c r="EA38" s="31"/>
+      <c r="EB38" s="31"/>
+      <c r="EC38" s="31"/>
+      <c r="ED38" s="31"/>
+      <c r="EE38" s="31"/>
+      <c r="EF38" s="31"/>
+      <c r="EG38" s="31"/>
+      <c r="EH38" s="31"/>
+      <c r="EI38" s="31"/>
+      <c r="EJ38" s="31"/>
+      <c r="EK38" s="31"/>
+      <c r="EL38" s="31"/>
+      <c r="EM38" s="31"/>
+      <c r="EN38" s="31"/>
+      <c r="EO38" s="31"/>
+      <c r="EP38" s="31"/>
+      <c r="EQ38" s="31"/>
+      <c r="ER38" s="31"/>
+      <c r="ES38" s="31"/>
+      <c r="ET38" s="31"/>
+      <c r="EU38" s="31"/>
+      <c r="EV38" s="31"/>
+      <c r="EW38" s="31"/>
+      <c r="EX38" s="31"/>
+      <c r="EY38" s="31"/>
+      <c r="EZ38" s="31"/>
+      <c r="FA38" s="31"/>
+      <c r="FB38" s="31"/>
+      <c r="FC38" s="31"/>
+      <c r="FD38" s="31"/>
+      <c r="FE38" s="31"/>
+      <c r="FF38" s="31"/>
+      <c r="FG38" s="31"/>
+      <c r="FH38" s="31"/>
+      <c r="FI38" s="31"/>
+      <c r="FJ38" s="31"/>
+      <c r="FK38" s="31"/>
+      <c r="FL38" s="31"/>
+      <c r="FM38" s="31"/>
+      <c r="FN38" s="31"/>
+      <c r="FO38" s="31"/>
+      <c r="FP38" s="31"/>
+      <c r="FQ38" s="31"/>
+      <c r="FR38" s="31"/>
+      <c r="FS38" s="31"/>
+      <c r="FT38" s="31"/>
+    </row>
+    <row r="39" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="45"/>
+      <c r="B39" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="60"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="83">
+        <v>44739</v>
+      </c>
+      <c r="F39" s="83">
+        <v>44745</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14">
+        <f t="shared" si="89"/>
+        <v>7</v>
+      </c>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="31"/>
+      <c r="V39" s="31"/>
+      <c r="W39" s="31"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="31"/>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
+      <c r="AF39" s="31"/>
+      <c r="AG39" s="31"/>
+      <c r="AH39" s="31"/>
+      <c r="AI39" s="31"/>
+      <c r="AJ39" s="31"/>
+      <c r="AK39" s="31"/>
+      <c r="AL39" s="31"/>
+      <c r="AM39" s="31"/>
+      <c r="AN39" s="31"/>
+      <c r="AO39" s="31"/>
+      <c r="AP39" s="31"/>
+      <c r="AQ39" s="31"/>
+      <c r="AR39" s="31"/>
+      <c r="AS39" s="31"/>
+      <c r="AT39" s="31"/>
+      <c r="AU39" s="31"/>
+      <c r="AV39" s="31"/>
+      <c r="AW39" s="31"/>
+      <c r="AX39" s="31"/>
+      <c r="AY39" s="31"/>
+      <c r="AZ39" s="31"/>
+      <c r="BA39" s="31"/>
+      <c r="BB39" s="31"/>
+      <c r="BC39" s="31"/>
+      <c r="BD39" s="31"/>
+      <c r="BE39" s="31"/>
+      <c r="BF39" s="31"/>
+      <c r="BG39" s="31"/>
+      <c r="BH39" s="31"/>
+      <c r="BI39" s="31"/>
+      <c r="BJ39" s="31"/>
+      <c r="BK39" s="31"/>
+      <c r="BL39" s="31"/>
+      <c r="BM39" s="31"/>
+      <c r="BN39" s="31"/>
+      <c r="BO39" s="31"/>
+      <c r="BP39" s="31"/>
+      <c r="BQ39" s="31"/>
+      <c r="BR39" s="31"/>
+      <c r="BS39" s="31"/>
+      <c r="BT39" s="31"/>
+      <c r="BU39" s="31"/>
+      <c r="BV39" s="31"/>
+      <c r="BW39" s="31"/>
+      <c r="BX39" s="31"/>
+      <c r="BY39" s="31"/>
+      <c r="BZ39" s="31"/>
+      <c r="CA39" s="31"/>
+      <c r="CB39" s="31"/>
+      <c r="CC39" s="31"/>
+      <c r="CD39" s="31"/>
+      <c r="CE39" s="31"/>
+      <c r="CF39" s="31"/>
+      <c r="CG39" s="31"/>
+      <c r="CH39" s="31"/>
+      <c r="CI39" s="31"/>
+      <c r="CJ39" s="31"/>
+      <c r="CK39" s="31"/>
+      <c r="CL39" s="31"/>
+      <c r="CM39" s="31"/>
+      <c r="CN39" s="31"/>
+      <c r="CO39" s="31"/>
+      <c r="CP39" s="31"/>
+      <c r="CQ39" s="31"/>
+      <c r="CR39" s="31"/>
+      <c r="CS39" s="31"/>
+      <c r="CT39" s="31"/>
+      <c r="CU39" s="31"/>
+      <c r="CV39" s="31"/>
+      <c r="CW39" s="31"/>
+      <c r="CX39" s="31"/>
+      <c r="CY39" s="31"/>
+      <c r="CZ39" s="31"/>
+      <c r="DA39" s="31"/>
+      <c r="DB39" s="31"/>
+      <c r="DC39" s="31"/>
+      <c r="DD39" s="31"/>
+      <c r="DE39" s="31"/>
+      <c r="DF39" s="31"/>
+      <c r="DG39" s="31"/>
+      <c r="DH39" s="31"/>
+      <c r="DI39" s="31"/>
+      <c r="DJ39" s="31"/>
+      <c r="DK39" s="31"/>
+      <c r="DL39" s="31"/>
+      <c r="DM39" s="31"/>
+      <c r="DN39" s="31"/>
+      <c r="DO39" s="31"/>
+      <c r="DP39" s="31"/>
+      <c r="DQ39" s="31"/>
+      <c r="DR39" s="31"/>
+      <c r="DS39" s="31"/>
+      <c r="DT39" s="31"/>
+      <c r="DU39" s="31"/>
+      <c r="DV39" s="31"/>
+      <c r="DW39" s="31"/>
+      <c r="DX39" s="31"/>
+      <c r="DY39" s="31"/>
+      <c r="DZ39" s="31"/>
+      <c r="EA39" s="31"/>
+      <c r="EB39" s="31"/>
+      <c r="EC39" s="31"/>
+      <c r="ED39" s="31"/>
+      <c r="EE39" s="31"/>
+      <c r="EF39" s="31"/>
+      <c r="EG39" s="31"/>
+      <c r="EH39" s="31"/>
+      <c r="EI39" s="31"/>
+      <c r="EJ39" s="31"/>
+      <c r="EK39" s="31"/>
+      <c r="EL39" s="31"/>
+      <c r="EM39" s="31"/>
+      <c r="EN39" s="31"/>
+      <c r="EO39" s="31"/>
+      <c r="EP39" s="31"/>
+      <c r="EQ39" s="31"/>
+      <c r="ER39" s="31"/>
+      <c r="ES39" s="31"/>
+      <c r="ET39" s="31"/>
+      <c r="EU39" s="31"/>
+      <c r="EV39" s="31"/>
+      <c r="EW39" s="31"/>
+      <c r="EX39" s="31"/>
+      <c r="EY39" s="31"/>
+      <c r="EZ39" s="31"/>
+      <c r="FA39" s="31"/>
+      <c r="FB39" s="31"/>
+      <c r="FC39" s="31"/>
+      <c r="FD39" s="31"/>
+      <c r="FE39" s="31"/>
+      <c r="FF39" s="31"/>
+      <c r="FG39" s="31"/>
+      <c r="FH39" s="31"/>
+      <c r="FI39" s="31"/>
+      <c r="FJ39" s="31"/>
+      <c r="FK39" s="31"/>
+      <c r="FL39" s="31"/>
+      <c r="FM39" s="31"/>
+      <c r="FN39" s="31"/>
+      <c r="FO39" s="31"/>
+      <c r="FP39" s="31"/>
+      <c r="FQ39" s="31"/>
+      <c r="FR39" s="31"/>
+      <c r="FS39" s="31"/>
+      <c r="FT39" s="31"/>
+    </row>
+    <row r="40" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="45"/>
+      <c r="B40" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="60"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="83">
+        <v>44746</v>
+      </c>
+      <c r="F40" s="83">
+        <v>44752</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14">
+        <f t="shared" si="89"/>
+        <v>7</v>
+      </c>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="31"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="31"/>
+      <c r="V40" s="31"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
+      <c r="AF40" s="31"/>
+      <c r="AG40" s="31"/>
+      <c r="AH40" s="31"/>
+      <c r="AI40" s="31"/>
+      <c r="AJ40" s="31"/>
+      <c r="AK40" s="31"/>
+      <c r="AL40" s="31"/>
+      <c r="AM40" s="31"/>
+      <c r="AN40" s="31"/>
+      <c r="AO40" s="31"/>
+      <c r="AP40" s="31"/>
+      <c r="AQ40" s="31"/>
+      <c r="AR40" s="31"/>
+      <c r="AS40" s="31"/>
+      <c r="AT40" s="31"/>
+      <c r="AU40" s="31"/>
+      <c r="AV40" s="31"/>
+      <c r="AW40" s="31"/>
+      <c r="AX40" s="31"/>
+      <c r="AY40" s="31"/>
+      <c r="AZ40" s="31"/>
+      <c r="BA40" s="31"/>
+      <c r="BB40" s="31"/>
+      <c r="BC40" s="31"/>
+      <c r="BD40" s="31"/>
+      <c r="BE40" s="31"/>
+      <c r="BF40" s="31"/>
+      <c r="BG40" s="31"/>
+      <c r="BH40" s="31"/>
+      <c r="BI40" s="31"/>
+      <c r="BJ40" s="31"/>
+      <c r="BK40" s="31"/>
+      <c r="BL40" s="31"/>
+      <c r="BM40" s="31"/>
+      <c r="BN40" s="31"/>
+      <c r="BO40" s="31"/>
+      <c r="BP40" s="31"/>
+      <c r="BQ40" s="31"/>
+      <c r="BR40" s="31"/>
+      <c r="BS40" s="31"/>
+      <c r="BT40" s="31"/>
+      <c r="BU40" s="31"/>
+      <c r="BV40" s="31"/>
+      <c r="BW40" s="31"/>
+      <c r="BX40" s="31"/>
+      <c r="BY40" s="31"/>
+      <c r="BZ40" s="31"/>
+      <c r="CA40" s="31"/>
+      <c r="CB40" s="31"/>
+      <c r="CC40" s="31"/>
+      <c r="CD40" s="31"/>
+      <c r="CE40" s="31"/>
+      <c r="CF40" s="31"/>
+      <c r="CG40" s="31"/>
+      <c r="CH40" s="31"/>
+      <c r="CI40" s="31"/>
+      <c r="CJ40" s="31"/>
+      <c r="CK40" s="31"/>
+      <c r="CL40" s="31"/>
+      <c r="CM40" s="31"/>
+      <c r="CN40" s="31"/>
+      <c r="CO40" s="31"/>
+      <c r="CP40" s="31"/>
+      <c r="CQ40" s="31"/>
+      <c r="CR40" s="31"/>
+      <c r="CS40" s="31"/>
+      <c r="CT40" s="31"/>
+      <c r="CU40" s="31"/>
+      <c r="CV40" s="31"/>
+      <c r="CW40" s="31"/>
+      <c r="CX40" s="31"/>
+      <c r="CY40" s="31"/>
+      <c r="CZ40" s="31"/>
+      <c r="DA40" s="31"/>
+      <c r="DB40" s="31"/>
+      <c r="DC40" s="31"/>
+      <c r="DD40" s="31"/>
+      <c r="DE40" s="31"/>
+      <c r="DF40" s="31"/>
+      <c r="DG40" s="31"/>
+      <c r="DH40" s="31"/>
+      <c r="DI40" s="31"/>
+      <c r="DJ40" s="31"/>
+      <c r="DK40" s="31"/>
+      <c r="DL40" s="31"/>
+      <c r="DM40" s="31"/>
+      <c r="DN40" s="31"/>
+      <c r="DO40" s="31"/>
+      <c r="DP40" s="31"/>
+      <c r="DQ40" s="31"/>
+      <c r="DR40" s="31"/>
+      <c r="DS40" s="31"/>
+      <c r="DT40" s="31"/>
+      <c r="DU40" s="31"/>
+      <c r="DV40" s="31"/>
+      <c r="DW40" s="31"/>
+      <c r="DX40" s="31"/>
+      <c r="DY40" s="31"/>
+      <c r="DZ40" s="31"/>
+      <c r="EA40" s="31"/>
+      <c r="EB40" s="31"/>
+      <c r="EC40" s="31"/>
+      <c r="ED40" s="31"/>
+      <c r="EE40" s="31"/>
+      <c r="EF40" s="31"/>
+      <c r="EG40" s="31"/>
+      <c r="EH40" s="31"/>
+      <c r="EI40" s="31"/>
+      <c r="EJ40" s="31"/>
+      <c r="EK40" s="31"/>
+      <c r="EL40" s="31"/>
+      <c r="EM40" s="31"/>
+      <c r="EN40" s="31"/>
+      <c r="EO40" s="31"/>
+      <c r="EP40" s="31"/>
+      <c r="EQ40" s="31"/>
+      <c r="ER40" s="31"/>
+      <c r="ES40" s="31"/>
+      <c r="ET40" s="31"/>
+      <c r="EU40" s="31"/>
+      <c r="EV40" s="31"/>
+      <c r="EW40" s="31"/>
+      <c r="EX40" s="31"/>
+      <c r="EY40" s="31"/>
+      <c r="EZ40" s="31"/>
+      <c r="FA40" s="31"/>
+      <c r="FB40" s="31"/>
+      <c r="FC40" s="31"/>
+      <c r="FD40" s="31"/>
+      <c r="FE40" s="31"/>
+      <c r="FF40" s="31"/>
+      <c r="FG40" s="31"/>
+      <c r="FH40" s="31"/>
+      <c r="FI40" s="31"/>
+      <c r="FJ40" s="31"/>
+      <c r="FK40" s="31"/>
+      <c r="FL40" s="31"/>
+      <c r="FM40" s="31"/>
+      <c r="FN40" s="31"/>
+      <c r="FO40" s="31"/>
+      <c r="FP40" s="31"/>
+      <c r="FQ40" s="31"/>
+      <c r="FR40" s="31"/>
+      <c r="FS40" s="31"/>
+      <c r="FT40" s="31"/>
+    </row>
+    <row r="41" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="66"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
-      <c r="Q38" s="33"/>
-      <c r="R38" s="33"/>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="33"/>
-      <c r="V38" s="33"/>
-      <c r="W38" s="33"/>
-      <c r="X38" s="33"/>
-      <c r="Y38" s="33"/>
-      <c r="Z38" s="33"/>
-      <c r="AA38" s="33"/>
-      <c r="AB38" s="33"/>
-      <c r="AC38" s="33"/>
-      <c r="AD38" s="33"/>
-      <c r="AE38" s="33"/>
-      <c r="AF38" s="33"/>
-      <c r="AG38" s="33"/>
-      <c r="AH38" s="33"/>
-      <c r="AI38" s="33"/>
-      <c r="AJ38" s="33"/>
-      <c r="AK38" s="33"/>
-      <c r="AL38" s="33"/>
-      <c r="AM38" s="33"/>
-      <c r="AN38" s="33"/>
-      <c r="AO38" s="33"/>
-      <c r="AP38" s="33"/>
-      <c r="AQ38" s="33"/>
-      <c r="AR38" s="33"/>
-      <c r="AS38" s="33"/>
-      <c r="AT38" s="33"/>
-      <c r="AU38" s="33"/>
-      <c r="AV38" s="33"/>
-      <c r="AW38" s="33"/>
-      <c r="AX38" s="33"/>
-      <c r="AY38" s="33"/>
-      <c r="AZ38" s="33"/>
-      <c r="BA38" s="33"/>
-      <c r="BB38" s="33"/>
-      <c r="BC38" s="33"/>
-      <c r="BD38" s="33"/>
-      <c r="BE38" s="33"/>
-      <c r="BF38" s="33"/>
-      <c r="BG38" s="33"/>
-      <c r="BH38" s="33"/>
-      <c r="BI38" s="33"/>
-      <c r="BJ38" s="33"/>
-      <c r="BK38" s="33"/>
-      <c r="BL38" s="33"/>
-      <c r="BM38" s="33"/>
-      <c r="BN38" s="33"/>
-      <c r="BO38" s="33"/>
-      <c r="BP38" s="33"/>
-      <c r="BQ38" s="33"/>
-      <c r="BR38" s="33"/>
-      <c r="BS38" s="33"/>
-      <c r="BT38" s="33"/>
-      <c r="BU38" s="33"/>
-      <c r="BV38" s="33"/>
-      <c r="BW38" s="33"/>
-      <c r="BX38" s="33"/>
-      <c r="BY38" s="33"/>
-      <c r="BZ38" s="33"/>
-      <c r="CA38" s="33"/>
-      <c r="CB38" s="33"/>
-      <c r="CC38" s="33"/>
-      <c r="CD38" s="33"/>
-      <c r="CE38" s="33"/>
-      <c r="CF38" s="33"/>
-      <c r="CG38" s="33"/>
-      <c r="CH38" s="33"/>
-      <c r="CI38" s="33"/>
-      <c r="CJ38" s="33"/>
-      <c r="CK38" s="33"/>
-      <c r="CL38" s="33"/>
-      <c r="CM38" s="33"/>
-      <c r="CN38" s="33"/>
-      <c r="CO38" s="33"/>
-      <c r="CP38" s="33"/>
-      <c r="CQ38" s="33"/>
-      <c r="CR38" s="33"/>
-      <c r="CS38" s="33"/>
-      <c r="CT38" s="33"/>
-      <c r="CU38" s="33"/>
-      <c r="CV38" s="33"/>
-      <c r="CW38" s="33"/>
-      <c r="CX38" s="33"/>
-      <c r="CY38" s="33"/>
-      <c r="CZ38" s="33"/>
-      <c r="DA38" s="33"/>
-      <c r="DB38" s="33"/>
-      <c r="DC38" s="33"/>
-      <c r="DD38" s="33"/>
-      <c r="DE38" s="33"/>
-      <c r="DF38" s="33"/>
-      <c r="DG38" s="33"/>
-      <c r="DH38" s="33"/>
-      <c r="DI38" s="33"/>
-      <c r="DJ38" s="33"/>
-      <c r="DK38" s="33"/>
-      <c r="DL38" s="33"/>
-      <c r="DM38" s="33"/>
-      <c r="DN38" s="33"/>
-      <c r="DO38" s="33"/>
-      <c r="DP38" s="33"/>
-      <c r="DQ38" s="33"/>
-      <c r="DR38" s="33"/>
-      <c r="DS38" s="33"/>
-      <c r="DT38" s="33"/>
-      <c r="DU38" s="33"/>
-      <c r="DV38" s="33"/>
-      <c r="DW38" s="33"/>
-      <c r="DX38" s="33"/>
-      <c r="DY38" s="33"/>
-      <c r="DZ38" s="33"/>
-      <c r="EA38" s="33"/>
-      <c r="EB38" s="33"/>
-      <c r="EC38" s="33"/>
-      <c r="ED38" s="33"/>
-      <c r="EE38" s="33"/>
-      <c r="EF38" s="33"/>
-      <c r="EG38" s="33"/>
-      <c r="EH38" s="33"/>
-      <c r="EI38" s="33"/>
-      <c r="EJ38" s="33"/>
-      <c r="EK38" s="33"/>
-      <c r="EL38" s="33"/>
-      <c r="EM38" s="33"/>
-      <c r="EN38" s="33"/>
-      <c r="EO38" s="33"/>
-      <c r="EP38" s="33"/>
-      <c r="EQ38" s="33"/>
-      <c r="ER38" s="33"/>
-      <c r="ES38" s="33"/>
-      <c r="ET38" s="33"/>
-      <c r="EU38" s="33"/>
-      <c r="EV38" s="33"/>
-      <c r="EW38" s="33"/>
-      <c r="EX38" s="33"/>
-      <c r="EY38" s="33"/>
-      <c r="EZ38" s="33"/>
-      <c r="FA38" s="33"/>
-      <c r="FB38" s="33"/>
-      <c r="FC38" s="33"/>
-      <c r="FD38" s="33"/>
-      <c r="FE38" s="33"/>
-      <c r="FF38" s="33"/>
-      <c r="FG38" s="33"/>
-      <c r="FH38" s="33"/>
-      <c r="FI38" s="33"/>
-      <c r="FJ38" s="33"/>
-      <c r="FK38" s="33"/>
-      <c r="FL38" s="33"/>
-      <c r="FM38" s="33"/>
-      <c r="FN38" s="33"/>
-      <c r="FO38" s="33"/>
-      <c r="FP38" s="33"/>
-      <c r="FQ38" s="33"/>
-      <c r="FR38" s="33"/>
-      <c r="FS38" s="33"/>
-      <c r="FT38" s="33"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
+      <c r="AF41" s="31"/>
+      <c r="AG41" s="31"/>
+      <c r="AH41" s="31"/>
+      <c r="AI41" s="31"/>
+      <c r="AJ41" s="31"/>
+      <c r="AK41" s="31"/>
+      <c r="AL41" s="31"/>
+      <c r="AM41" s="31"/>
+      <c r="AN41" s="31"/>
+      <c r="AO41" s="31"/>
+      <c r="AP41" s="31"/>
+      <c r="AQ41" s="31"/>
+      <c r="AR41" s="31"/>
+      <c r="AS41" s="31"/>
+      <c r="AT41" s="31"/>
+      <c r="AU41" s="31"/>
+      <c r="AV41" s="31"/>
+      <c r="AW41" s="31"/>
+      <c r="AX41" s="31"/>
+      <c r="AY41" s="31"/>
+      <c r="AZ41" s="31"/>
+      <c r="BA41" s="31"/>
+      <c r="BB41" s="31"/>
+      <c r="BC41" s="31"/>
+      <c r="BD41" s="31"/>
+      <c r="BE41" s="31"/>
+      <c r="BF41" s="31"/>
+      <c r="BG41" s="31"/>
+      <c r="BH41" s="31"/>
+      <c r="BI41" s="31"/>
+      <c r="BJ41" s="31"/>
+      <c r="BK41" s="31"/>
+      <c r="BL41" s="31"/>
+      <c r="BM41" s="31"/>
+      <c r="BN41" s="31"/>
+      <c r="BO41" s="31"/>
+      <c r="BP41" s="31"/>
+      <c r="BQ41" s="31"/>
+      <c r="BR41" s="31"/>
+      <c r="BS41" s="31"/>
+      <c r="BT41" s="31"/>
+      <c r="BU41" s="31"/>
+      <c r="BV41" s="31"/>
+      <c r="BW41" s="31"/>
+      <c r="BX41" s="31"/>
+      <c r="BY41" s="31"/>
+      <c r="BZ41" s="31"/>
+      <c r="CA41" s="31"/>
+      <c r="CB41" s="31"/>
+      <c r="CC41" s="31"/>
+      <c r="CD41" s="31"/>
+      <c r="CE41" s="31"/>
+      <c r="CF41" s="31"/>
+      <c r="CG41" s="31"/>
+      <c r="CH41" s="31"/>
+      <c r="CI41" s="31"/>
+      <c r="CJ41" s="31"/>
+      <c r="CK41" s="31"/>
+      <c r="CL41" s="31"/>
+      <c r="CM41" s="31"/>
+      <c r="CN41" s="31"/>
+      <c r="CO41" s="31"/>
+      <c r="CP41" s="31"/>
+      <c r="CQ41" s="31"/>
+      <c r="CR41" s="31"/>
+      <c r="CS41" s="31"/>
+      <c r="CT41" s="31"/>
+      <c r="CU41" s="31"/>
+      <c r="CV41" s="31"/>
+      <c r="CW41" s="31"/>
+      <c r="CX41" s="31"/>
+      <c r="CY41" s="31"/>
+      <c r="CZ41" s="31"/>
+      <c r="DA41" s="31"/>
+      <c r="DB41" s="31"/>
+      <c r="DC41" s="31"/>
+      <c r="DD41" s="31"/>
+      <c r="DE41" s="31"/>
+      <c r="DF41" s="31"/>
+      <c r="DG41" s="31"/>
+      <c r="DH41" s="31"/>
+      <c r="DI41" s="31"/>
+      <c r="DJ41" s="31"/>
+      <c r="DK41" s="31"/>
+      <c r="DL41" s="31"/>
+      <c r="DM41" s="31"/>
+      <c r="DN41" s="31"/>
+      <c r="DO41" s="31"/>
+      <c r="DP41" s="31"/>
+      <c r="DQ41" s="31"/>
+      <c r="DR41" s="31"/>
+      <c r="DS41" s="31"/>
+      <c r="DT41" s="31"/>
+      <c r="DU41" s="31"/>
+      <c r="DV41" s="31"/>
+      <c r="DW41" s="31"/>
+      <c r="DX41" s="31"/>
+      <c r="DY41" s="31"/>
+      <c r="DZ41" s="31"/>
+      <c r="EA41" s="31"/>
+      <c r="EB41" s="31"/>
+      <c r="EC41" s="31"/>
+      <c r="ED41" s="31"/>
+      <c r="EE41" s="31"/>
+      <c r="EF41" s="31"/>
+      <c r="EG41" s="31"/>
+      <c r="EH41" s="31"/>
+      <c r="EI41" s="31"/>
+      <c r="EJ41" s="31"/>
+      <c r="EK41" s="31"/>
+      <c r="EL41" s="31"/>
+      <c r="EM41" s="31"/>
+      <c r="EN41" s="31"/>
+      <c r="EO41" s="31"/>
+      <c r="EP41" s="31"/>
+      <c r="EQ41" s="31"/>
+      <c r="ER41" s="31"/>
+      <c r="ES41" s="31"/>
+      <c r="ET41" s="31"/>
+      <c r="EU41" s="31"/>
+      <c r="EV41" s="31"/>
+      <c r="EW41" s="31"/>
+      <c r="EX41" s="31"/>
+      <c r="EY41" s="31"/>
+      <c r="EZ41" s="31"/>
+      <c r="FA41" s="31"/>
+      <c r="FB41" s="31"/>
+      <c r="FC41" s="31"/>
+      <c r="FD41" s="31"/>
+      <c r="FE41" s="31"/>
+      <c r="FF41" s="31"/>
+      <c r="FG41" s="31"/>
+      <c r="FH41" s="31"/>
+      <c r="FI41" s="31"/>
+      <c r="FJ41" s="31"/>
+      <c r="FK41" s="31"/>
+      <c r="FL41" s="31"/>
+      <c r="FM41" s="31"/>
+      <c r="FN41" s="31"/>
+      <c r="FO41" s="31"/>
+      <c r="FP41" s="31"/>
+      <c r="FQ41" s="31"/>
+      <c r="FR41" s="31"/>
+      <c r="FS41" s="31"/>
+      <c r="FT41" s="31"/>
     </row>
-    <row r="39" spans="1:176" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G39" s="6"/>
+    <row r="42" spans="1:176" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="75"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30" t="str">
+        <f t="shared" si="89"/>
+        <v/>
+      </c>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="33"/>
+      <c r="S42" s="33"/>
+      <c r="T42" s="33"/>
+      <c r="U42" s="33"/>
+      <c r="V42" s="33"/>
+      <c r="W42" s="33"/>
+      <c r="X42" s="33"/>
+      <c r="Y42" s="33"/>
+      <c r="Z42" s="33"/>
+      <c r="AA42" s="33"/>
+      <c r="AB42" s="33"/>
+      <c r="AC42" s="33"/>
+      <c r="AD42" s="33"/>
+      <c r="AE42" s="33"/>
+      <c r="AF42" s="33"/>
+      <c r="AG42" s="33"/>
+      <c r="AH42" s="33"/>
+      <c r="AI42" s="33"/>
+      <c r="AJ42" s="33"/>
+      <c r="AK42" s="33"/>
+      <c r="AL42" s="33"/>
+      <c r="AM42" s="33"/>
+      <c r="AN42" s="33"/>
+      <c r="AO42" s="33"/>
+      <c r="AP42" s="33"/>
+      <c r="AQ42" s="33"/>
+      <c r="AR42" s="33"/>
+      <c r="AS42" s="33"/>
+      <c r="AT42" s="33"/>
+      <c r="AU42" s="33"/>
+      <c r="AV42" s="33"/>
+      <c r="AW42" s="33"/>
+      <c r="AX42" s="33"/>
+      <c r="AY42" s="33"/>
+      <c r="AZ42" s="33"/>
+      <c r="BA42" s="33"/>
+      <c r="BB42" s="33"/>
+      <c r="BC42" s="33"/>
+      <c r="BD42" s="33"/>
+      <c r="BE42" s="33"/>
+      <c r="BF42" s="33"/>
+      <c r="BG42" s="33"/>
+      <c r="BH42" s="33"/>
+      <c r="BI42" s="33"/>
+      <c r="BJ42" s="33"/>
+      <c r="BK42" s="33"/>
+      <c r="BL42" s="33"/>
+      <c r="BM42" s="33"/>
+      <c r="BN42" s="33"/>
+      <c r="BO42" s="33"/>
+      <c r="BP42" s="33"/>
+      <c r="BQ42" s="33"/>
+      <c r="BR42" s="33"/>
+      <c r="BS42" s="33"/>
+      <c r="BT42" s="33"/>
+      <c r="BU42" s="33"/>
+      <c r="BV42" s="33"/>
+      <c r="BW42" s="33"/>
+      <c r="BX42" s="33"/>
+      <c r="BY42" s="33"/>
+      <c r="BZ42" s="33"/>
+      <c r="CA42" s="33"/>
+      <c r="CB42" s="33"/>
+      <c r="CC42" s="33"/>
+      <c r="CD42" s="33"/>
+      <c r="CE42" s="33"/>
+      <c r="CF42" s="33"/>
+      <c r="CG42" s="33"/>
+      <c r="CH42" s="33"/>
+      <c r="CI42" s="33"/>
+      <c r="CJ42" s="33"/>
+      <c r="CK42" s="33"/>
+      <c r="CL42" s="33"/>
+      <c r="CM42" s="33"/>
+      <c r="CN42" s="33"/>
+      <c r="CO42" s="33"/>
+      <c r="CP42" s="33"/>
+      <c r="CQ42" s="33"/>
+      <c r="CR42" s="33"/>
+      <c r="CS42" s="33"/>
+      <c r="CT42" s="33"/>
+      <c r="CU42" s="33"/>
+      <c r="CV42" s="33"/>
+      <c r="CW42" s="33"/>
+      <c r="CX42" s="33"/>
+      <c r="CY42" s="33"/>
+      <c r="CZ42" s="33"/>
+      <c r="DA42" s="33"/>
+      <c r="DB42" s="33"/>
+      <c r="DC42" s="33"/>
+      <c r="DD42" s="33"/>
+      <c r="DE42" s="33"/>
+      <c r="DF42" s="33"/>
+      <c r="DG42" s="33"/>
+      <c r="DH42" s="33"/>
+      <c r="DI42" s="33"/>
+      <c r="DJ42" s="33"/>
+      <c r="DK42" s="33"/>
+      <c r="DL42" s="33"/>
+      <c r="DM42" s="33"/>
+      <c r="DN42" s="33"/>
+      <c r="DO42" s="33"/>
+      <c r="DP42" s="33"/>
+      <c r="DQ42" s="33"/>
+      <c r="DR42" s="33"/>
+      <c r="DS42" s="33"/>
+      <c r="DT42" s="33"/>
+      <c r="DU42" s="33"/>
+      <c r="DV42" s="33"/>
+      <c r="DW42" s="33"/>
+      <c r="DX42" s="33"/>
+      <c r="DY42" s="33"/>
+      <c r="DZ42" s="33"/>
+      <c r="EA42" s="33"/>
+      <c r="EB42" s="33"/>
+      <c r="EC42" s="33"/>
+      <c r="ED42" s="33"/>
+      <c r="EE42" s="33"/>
+      <c r="EF42" s="33"/>
+      <c r="EG42" s="33"/>
+      <c r="EH42" s="33"/>
+      <c r="EI42" s="33"/>
+      <c r="EJ42" s="33"/>
+      <c r="EK42" s="33"/>
+      <c r="EL42" s="33"/>
+      <c r="EM42" s="33"/>
+      <c r="EN42" s="33"/>
+      <c r="EO42" s="33"/>
+      <c r="EP42" s="33"/>
+      <c r="EQ42" s="33"/>
+      <c r="ER42" s="33"/>
+      <c r="ES42" s="33"/>
+      <c r="ET42" s="33"/>
+      <c r="EU42" s="33"/>
+      <c r="EV42" s="33"/>
+      <c r="EW42" s="33"/>
+      <c r="EX42" s="33"/>
+      <c r="EY42" s="33"/>
+      <c r="EZ42" s="33"/>
+      <c r="FA42" s="33"/>
+      <c r="FB42" s="33"/>
+      <c r="FC42" s="33"/>
+      <c r="FD42" s="33"/>
+      <c r="FE42" s="33"/>
+      <c r="FF42" s="33"/>
+      <c r="FG42" s="33"/>
+      <c r="FH42" s="33"/>
+      <c r="FI42" s="33"/>
+      <c r="FJ42" s="33"/>
+      <c r="FK42" s="33"/>
+      <c r="FL42" s="33"/>
+      <c r="FM42" s="33"/>
+      <c r="FN42" s="33"/>
+      <c r="FO42" s="33"/>
+      <c r="FP42" s="33"/>
+      <c r="FQ42" s="33"/>
+      <c r="FR42" s="33"/>
+      <c r="FS42" s="33"/>
+      <c r="FT42" s="33"/>
     </row>
-    <row r="40" spans="1:176" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="11"/>
-      <c r="F40" s="47"/>
+    <row r="43" spans="1:176" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G43" s="6"/>
     </row>
-    <row r="41" spans="1:176" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="12"/>
+    <row r="44" spans="1:176" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="11"/>
+      <c r="F44" s="47"/>
+    </row>
+    <row r="45" spans="1:176" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="FN5:FT5"/>
-    <mergeCell ref="EE5:EK5"/>
-    <mergeCell ref="EL5:ER5"/>
-    <mergeCell ref="ES5:EY5"/>
-    <mergeCell ref="EZ5:FF5"/>
-    <mergeCell ref="FG5:FM5"/>
-    <mergeCell ref="CV5:DB5"/>
-    <mergeCell ref="DC5:DI5"/>
-    <mergeCell ref="DJ5:DP5"/>
-    <mergeCell ref="DQ5:DW5"/>
-    <mergeCell ref="DX5:ED5"/>
-    <mergeCell ref="BM5:BS5"/>
-    <mergeCell ref="BT5:BZ5"/>
-    <mergeCell ref="CA5:CG5"/>
-    <mergeCell ref="CH5:CN5"/>
-    <mergeCell ref="CO5:CU5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="AK5:AQ5"/>
-    <mergeCell ref="AR5:AX5"/>
     <mergeCell ref="AY5:BE5"/>
     <mergeCell ref="BF5:BL5"/>
     <mergeCell ref="E3:F3"/>
@@ -9556,8 +10310,29 @@
     <mergeCell ref="P5:V5"/>
     <mergeCell ref="W5:AC5"/>
     <mergeCell ref="AD5:AJ5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="AK5:AQ5"/>
+    <mergeCell ref="AR5:AX5"/>
+    <mergeCell ref="BM5:BS5"/>
+    <mergeCell ref="BT5:BZ5"/>
+    <mergeCell ref="CA5:CG5"/>
+    <mergeCell ref="CH5:CN5"/>
+    <mergeCell ref="CO5:CU5"/>
+    <mergeCell ref="CV5:DB5"/>
+    <mergeCell ref="DC5:DI5"/>
+    <mergeCell ref="DJ5:DP5"/>
+    <mergeCell ref="DQ5:DW5"/>
+    <mergeCell ref="DX5:ED5"/>
+    <mergeCell ref="FN5:FT5"/>
+    <mergeCell ref="EE5:EK5"/>
+    <mergeCell ref="EL5:ER5"/>
+    <mergeCell ref="ES5:EY5"/>
+    <mergeCell ref="EZ5:FF5"/>
+    <mergeCell ref="FG5:FM5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D8:D38">
+  <conditionalFormatting sqref="D8:D42">
     <cfRule type="dataBar" priority="38">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9571,12 +10346,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6:BL38 FN6:FS38">
+  <conditionalFormatting sqref="I6:BL42 FN6:FS42">
     <cfRule type="expression" dxfId="20" priority="57">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:BL38 FN8:FS38">
+  <conditionalFormatting sqref="I8:BL42 FN8:FS42">
     <cfRule type="expression" dxfId="19" priority="51">
       <formula>AND(task_start&lt;=I$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$6)</formula>
     </cfRule>
@@ -9584,12 +10359,12 @@
       <formula>AND(task_end&gt;=I$6,task_start&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM6:CG38">
+  <conditionalFormatting sqref="BM6:CG42">
     <cfRule type="expression" dxfId="17" priority="24">
       <formula>AND(TODAY()&gt;=BM$6,TODAY()&lt;BN$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM8:CG38">
+  <conditionalFormatting sqref="BM8:CG42">
     <cfRule type="expression" dxfId="16" priority="22">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -9597,12 +10372,12 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BN$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH6:DB38">
+  <conditionalFormatting sqref="CH6:DB42">
     <cfRule type="expression" dxfId="14" priority="18">
       <formula>AND(TODAY()&gt;=CH$6,TODAY()&lt;CI$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH8:DB38">
+  <conditionalFormatting sqref="CH8:DB42">
     <cfRule type="expression" dxfId="13" priority="16">
       <formula>AND(task_start&lt;=CH$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$6)</formula>
     </cfRule>
@@ -9610,12 +10385,12 @@
       <formula>AND(task_end&gt;=CH$6,task_start&lt;CI$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DC6:DW38">
+  <conditionalFormatting sqref="DC6:DW42">
     <cfRule type="expression" dxfId="11" priority="15">
       <formula>AND(TODAY()&gt;=DC$6,TODAY()&lt;DD$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DC8:DW38">
+  <conditionalFormatting sqref="DC8:DW42">
     <cfRule type="expression" dxfId="10" priority="13">
       <formula>AND(task_start&lt;=DC$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=DC$6)</formula>
     </cfRule>
@@ -9623,12 +10398,12 @@
       <formula>AND(task_end&gt;=DC$6,task_start&lt;DD$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DX6:ER38">
+  <conditionalFormatting sqref="DX6:ER42">
     <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND(TODAY()&gt;=DX$6,TODAY()&lt;DY$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DX8:ER38">
+  <conditionalFormatting sqref="DX8:ER42">
     <cfRule type="expression" dxfId="7" priority="7">
       <formula>AND(task_start&lt;=DX$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=DX$6)</formula>
     </cfRule>
@@ -9636,12 +10411,12 @@
       <formula>AND(task_end&gt;=DX$6,task_start&lt;DY$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="ES6:FM38">
+  <conditionalFormatting sqref="ES6:FM42">
     <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(TODAY()&gt;=ES$6,TODAY()&lt;ET$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="ES8:FM38">
+  <conditionalFormatting sqref="ES8:FM42">
     <cfRule type="expression" dxfId="4" priority="4">
       <formula>AND(task_start&lt;=ES$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=ES$6)</formula>
     </cfRule>
@@ -9649,12 +10424,12 @@
       <formula>AND(task_end&gt;=ES$6,task_start&lt;ET$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FT6:FT38">
+  <conditionalFormatting sqref="FT6:FT42">
     <cfRule type="expression" dxfId="2" priority="59">
       <formula>AND(TODAY()&gt;=FT$6,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FT8:FT38">
+  <conditionalFormatting sqref="FT8:FT42">
     <cfRule type="expression" dxfId="1" priority="62">
       <formula>AND(task_start&lt;=FT$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=FT$6)</formula>
     </cfRule>
@@ -9689,7 +10464,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D8:D38</xm:sqref>
+          <xm:sqref>D8:D42</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>